<commit_message>
adding all parties data
</commit_message>
<xml_diff>
--- a/data/Laura Project application/Deputy + parties/party info participated in mun election/party sheets.xlsx
+++ b/data/Laura Project application/Deputy + parties/party info participated in mun election/party sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\office\Desktop\DI\internal_viz\data\Laura Project application\Deputy + parties\party info participated in mun election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140000_{0C7418CB-F288-4CAA-81F0-F48419C1ACC6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140000_{1BB46BCC-DBC6-4C55-AA83-B975DEA81E35}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5884" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5911" uniqueCount="758">
   <si>
     <t>mun_fr</t>
   </si>
@@ -4223,8 +4223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4277,462 +4277,462 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>119</v>
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>117</v>
+        <v>755</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>756</v>
       </c>
       <c r="F2">
-        <v>859</v>
+        <v>273</v>
       </c>
       <c r="G2">
-        <v>0.1598139534883721</v>
+        <v>2.298173246906305E-2</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>15743</v>
+        <v>46708</v>
       </c>
       <c r="J2">
-        <v>171</v>
+        <v>536</v>
       </c>
       <c r="K2">
-        <v>131</v>
+        <v>246</v>
       </c>
       <c r="L2">
-        <v>5375</v>
+        <v>11879</v>
       </c>
       <c r="M2">
-        <v>5677</v>
+        <v>12661</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3">
-        <v>286</v>
-      </c>
-      <c r="G3">
-        <v>0.13185799907791609</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>6922</v>
-      </c>
-      <c r="J3">
-        <v>147</v>
-      </c>
-      <c r="K3">
-        <v>68</v>
-      </c>
-      <c r="L3">
-        <v>2169</v>
-      </c>
-      <c r="M3">
-        <v>2384</v>
+      <c r="A3" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>755</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="F3" s="20">
+        <v>230</v>
+      </c>
+      <c r="G3" s="20">
+        <v>1.573187414500684E-2</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0</v>
+      </c>
+      <c r="I3" s="20">
+        <v>50600</v>
+      </c>
+      <c r="J3" s="20">
+        <v>325</v>
+      </c>
+      <c r="K3" s="20">
+        <v>195</v>
+      </c>
+      <c r="L3" s="20">
+        <v>14620</v>
+      </c>
+      <c r="M3" s="20">
+        <v>15140</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>301</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>303</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F4">
-        <v>1091</v>
-      </c>
-      <c r="G4">
-        <v>3.714421898406646E-2</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>76783</v>
-      </c>
-      <c r="J4">
-        <v>456</v>
-      </c>
-      <c r="K4">
-        <v>335</v>
-      </c>
-      <c r="L4">
-        <v>29372</v>
-      </c>
-      <c r="M4">
-        <v>30163</v>
+      <c r="A4" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>755</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="F4" s="20">
+        <v>283</v>
+      </c>
+      <c r="G4" s="20">
+        <v>4.1199592371524242E-2</v>
+      </c>
+      <c r="H4" s="20">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20">
+        <v>20443</v>
+      </c>
+      <c r="J4" s="20">
+        <v>297</v>
+      </c>
+      <c r="K4" s="20">
+        <v>142</v>
+      </c>
+      <c r="L4" s="20">
+        <v>6869</v>
+      </c>
+      <c r="M4" s="20">
+        <v>7308</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>262</v>
+        <v>202</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>263</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>303</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>304</v>
+        <v>755</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>756</v>
       </c>
       <c r="F5">
-        <v>263</v>
+        <v>331</v>
       </c>
       <c r="G5">
-        <v>2.5073886929163881E-2</v>
+        <v>2.2889150127930299E-2</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>41646</v>
+        <v>51010</v>
       </c>
       <c r="J5">
-        <v>586</v>
+        <v>261</v>
       </c>
       <c r="K5">
-        <v>314</v>
+        <v>251</v>
       </c>
       <c r="L5">
-        <v>10489</v>
+        <v>14461</v>
       </c>
       <c r="M5">
-        <v>11389</v>
+        <v>14973</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F6" s="20">
-        <v>791</v>
-      </c>
-      <c r="G6" s="20">
-        <v>4.1712809154669621E-2</v>
-      </c>
-      <c r="H6" s="20">
+      <c r="A6" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>755</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="F6">
+        <v>142</v>
+      </c>
+      <c r="G6">
+        <v>6.5558633425669435E-2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>7818</v>
+      </c>
+      <c r="J6">
+        <v>71</v>
+      </c>
+      <c r="K6">
+        <v>39</v>
+      </c>
+      <c r="L6">
+        <v>2166</v>
+      </c>
+      <c r="M6">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>755</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="F7">
+        <v>144</v>
+      </c>
+      <c r="G7">
+        <v>7.7544426494345717E-2</v>
+      </c>
+      <c r="H7" s="6">
         <v>2</v>
       </c>
-      <c r="I6" s="20">
-        <v>80820</v>
-      </c>
-      <c r="J6" s="20">
-        <v>950</v>
-      </c>
-      <c r="K6" s="20">
-        <v>445</v>
-      </c>
-      <c r="L6" s="20">
-        <v>18963</v>
-      </c>
-      <c r="M6" s="20">
-        <v>20358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>303</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F7">
-        <v>337</v>
-      </c>
-      <c r="G7">
-        <v>0.11056430446194231</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
       <c r="I7">
-        <v>6237</v>
+        <v>7670</v>
       </c>
       <c r="J7">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="K7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L7">
-        <v>3048</v>
+        <v>1857</v>
       </c>
       <c r="M7">
-        <v>3213</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>305</v>
+        <v>398</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>306</v>
+        <v>399</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
+        <v>755</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="F8">
+        <v>296</v>
+      </c>
+      <c r="G8">
+        <v>2.91453328081922E-2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>49945</v>
+      </c>
+      <c r="J8">
+        <v>579</v>
+      </c>
+      <c r="K8">
         <v>303</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F8">
-        <v>1105</v>
-      </c>
-      <c r="G8">
-        <v>8.4454295322531334E-2</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>44901</v>
-      </c>
-      <c r="J8">
-        <v>329</v>
-      </c>
-      <c r="K8">
-        <v>209</v>
-      </c>
       <c r="L8">
-        <v>13084</v>
+        <v>10156</v>
       </c>
       <c r="M8">
-        <v>13622</v>
+        <v>11038</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>313</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>314</v>
+      <c r="A9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>303</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>304</v>
+        <v>755</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>756</v>
       </c>
       <c r="F9">
-        <v>357</v>
+        <v>132</v>
       </c>
       <c r="G9">
-        <v>4.669718770438195E-2</v>
+        <v>2.25718194254446E-2</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>29721</v>
+        <v>15764</v>
       </c>
       <c r="J9">
-        <v>401</v>
+        <v>91</v>
       </c>
       <c r="K9">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="L9">
-        <v>7645</v>
+        <v>5848</v>
       </c>
       <c r="M9">
-        <v>8220</v>
+        <v>6032</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>195</v>
+      <c r="A10" t="s">
+        <v>538</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>303</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>304</v>
+        <v>755</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>756</v>
       </c>
       <c r="F10">
-        <v>3549</v>
+        <v>129</v>
       </c>
       <c r="G10">
-        <v>7.8092681424107732E-2</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
+        <v>1.3188835497392901E-2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>148647</v>
+        <v>25874</v>
       </c>
       <c r="J10">
-        <v>1007</v>
+        <v>229</v>
       </c>
       <c r="K10">
-        <v>784</v>
+        <v>99</v>
       </c>
       <c r="L10">
-        <v>45446</v>
+        <v>9781</v>
       </c>
       <c r="M10">
-        <v>47237</v>
+        <v>10109</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>256</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>183</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>303</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>304</v>
+        <v>755</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>756</v>
       </c>
       <c r="F11">
-        <v>1488</v>
+        <v>109</v>
       </c>
       <c r="G11">
-        <v>4.9580167932826873E-2</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
+        <v>6.2439136163143722E-3</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>102744</v>
+        <v>46430</v>
       </c>
       <c r="J11">
-        <v>921</v>
+        <v>384</v>
       </c>
       <c r="K11">
-        <v>561</v>
+        <v>209</v>
       </c>
       <c r="L11">
-        <v>30012</v>
+        <v>17457</v>
       </c>
       <c r="M11">
-        <v>31494</v>
+        <v>18050</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>310</v>
+        <v>448</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>449</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>303</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>304</v>
+        <v>755</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>756</v>
       </c>
       <c r="F12">
-        <v>116</v>
+        <v>261</v>
       </c>
       <c r="G12">
-        <v>3.9375424304141211E-2</v>
+        <v>3.076741718731581E-2</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>9975</v>
+        <v>38119</v>
       </c>
       <c r="J12">
-        <v>258</v>
+        <v>392</v>
       </c>
       <c r="K12">
-        <v>64</v>
-      </c>
-      <c r="L12">
-        <v>2946</v>
-      </c>
-      <c r="M12">
-        <v>3268</v>
+        <v>296</v>
+      </c>
+      <c r="L12" s="5">
+        <v>8484</v>
+      </c>
+      <c r="M12" s="5">
+        <v>9172</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>339</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>159</v>
+        <v>340</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -4744,1348 +4744,1348 @@
         <v>756</v>
       </c>
       <c r="F13">
-        <v>273</v>
+        <v>111</v>
       </c>
       <c r="G13">
-        <v>2.298173246906305E-2</v>
-      </c>
-      <c r="H13">
+        <v>1.261363636363636E-2</v>
+      </c>
+      <c r="H13" s="6">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>46708</v>
+        <v>37780</v>
       </c>
       <c r="J13">
-        <v>536</v>
+        <v>211</v>
       </c>
       <c r="K13">
-        <v>246</v>
+        <v>153</v>
       </c>
       <c r="L13">
-        <v>11879</v>
+        <v>8800</v>
       </c>
       <c r="M13">
-        <v>12661</v>
+        <v>9164</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="20" t="s">
+      <c r="A14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
         <v>755</v>
       </c>
       <c r="E14" s="24" t="s">
         <v>756</v>
       </c>
-      <c r="F14" s="20">
-        <v>230</v>
-      </c>
-      <c r="G14" s="20">
-        <v>1.573187414500684E-2</v>
-      </c>
-      <c r="H14" s="20">
-        <v>0</v>
-      </c>
-      <c r="I14" s="20">
-        <v>50600</v>
-      </c>
-      <c r="J14" s="20">
-        <v>325</v>
-      </c>
-      <c r="K14" s="20">
-        <v>195</v>
-      </c>
-      <c r="L14" s="20">
-        <v>14620</v>
-      </c>
-      <c r="M14" s="20">
-        <v>15140</v>
+      <c r="F14">
+        <v>232</v>
+      </c>
+      <c r="G14">
+        <v>3.0382399161864849E-2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>17748</v>
+      </c>
+      <c r="J14">
+        <v>170</v>
+      </c>
+      <c r="K14">
+        <v>79</v>
+      </c>
+      <c r="L14">
+        <v>7636</v>
+      </c>
+      <c r="M14">
+        <v>7885</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="A15" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
         <v>755</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>756</v>
       </c>
-      <c r="F15" s="20">
-        <v>283</v>
-      </c>
-      <c r="G15" s="20">
-        <v>4.1199592371524242E-2</v>
-      </c>
-      <c r="H15" s="20">
+      <c r="F15">
+        <v>149</v>
+      </c>
+      <c r="G15">
+        <v>1.7626878031468118E-2</v>
+      </c>
+      <c r="H15" s="6">
         <v>0</v>
       </c>
-      <c r="I15" s="20">
-        <v>20443</v>
-      </c>
-      <c r="J15" s="20">
-        <v>297</v>
-      </c>
-      <c r="K15" s="20">
-        <v>142</v>
-      </c>
-      <c r="L15" s="20">
-        <v>6869</v>
-      </c>
-      <c r="M15" s="20">
-        <v>7308</v>
+      <c r="I15">
+        <v>27942</v>
+      </c>
+      <c r="J15">
+        <v>279</v>
+      </c>
+      <c r="K15">
+        <v>167</v>
+      </c>
+      <c r="L15">
+        <v>8453</v>
+      </c>
+      <c r="M15">
+        <v>8899</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="A16" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>755</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>756</v>
       </c>
-      <c r="F16">
-        <v>331</v>
-      </c>
-      <c r="G16">
-        <v>2.2889150127930299E-2</v>
-      </c>
-      <c r="H16">
+      <c r="F16" s="20">
+        <v>1384</v>
+      </c>
+      <c r="G16" s="20">
+        <v>1.7393708605110029E-2</v>
+      </c>
+      <c r="H16" s="23">
         <v>0</v>
       </c>
-      <c r="I16">
-        <v>51010</v>
-      </c>
-      <c r="J16">
-        <v>261</v>
-      </c>
-      <c r="K16">
-        <v>251</v>
-      </c>
-      <c r="L16">
-        <v>14461</v>
-      </c>
-      <c r="M16">
-        <v>14973</v>
+      <c r="I16" s="20">
+        <v>328134</v>
+      </c>
+      <c r="J16" s="20">
+        <v>2831</v>
+      </c>
+      <c r="K16" s="20">
+        <v>2058</v>
+      </c>
+      <c r="L16" s="20">
+        <v>79569</v>
+      </c>
+      <c r="M16" s="20">
+        <v>84458</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>684</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>755</v>
+      <c r="A17" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="F17">
-        <v>142</v>
-      </c>
-      <c r="G17">
-        <v>6.5558633425669435E-2</v>
-      </c>
-      <c r="H17" s="6">
+        <v>744</v>
+      </c>
+      <c r="F17" s="17">
+        <v>319</v>
+      </c>
+      <c r="G17" s="17">
+        <v>6.8308351177730195E-2</v>
+      </c>
+      <c r="H17" s="17">
+        <v>2</v>
+      </c>
+      <c r="I17" s="17">
+        <v>12970</v>
+      </c>
+      <c r="J17" s="17">
+        <v>209</v>
+      </c>
+      <c r="K17" s="17">
+        <v>92</v>
+      </c>
+      <c r="L17" s="17">
+        <v>4670</v>
+      </c>
+      <c r="M17" s="17">
+        <v>4971</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>608</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>290</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F18">
+        <v>155</v>
+      </c>
+      <c r="G18">
+        <v>6.9851284362325378E-2</v>
+      </c>
+      <c r="H18" s="6">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>7818</v>
-      </c>
-      <c r="J17">
-        <v>71</v>
-      </c>
-      <c r="K17">
-        <v>39</v>
-      </c>
-      <c r="L17">
-        <v>2166</v>
-      </c>
-      <c r="M17">
-        <v>2276</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>755</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="F18">
-        <v>144</v>
-      </c>
-      <c r="G18">
-        <v>7.7544426494345717E-2</v>
-      </c>
-      <c r="H18" s="6">
-        <v>2</v>
-      </c>
       <c r="I18">
-        <v>7670</v>
+        <v>5031</v>
       </c>
       <c r="J18">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="K18">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L18">
-        <v>1857</v>
+        <v>2219</v>
       </c>
       <c r="M18">
-        <v>1993</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>398</v>
+        <v>736</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>399</v>
+        <v>737</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>755</v>
+        <v>290</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>756</v>
+        <v>744</v>
       </c>
       <c r="F19">
-        <v>296</v>
+        <v>149</v>
       </c>
       <c r="G19">
-        <v>2.91453328081922E-2</v>
-      </c>
-      <c r="H19" s="6">
-        <v>0</v>
+        <v>4.4305679452869458E-2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>49945</v>
+        <v>10945</v>
       </c>
       <c r="J19">
-        <v>579</v>
+        <v>269</v>
       </c>
       <c r="K19">
-        <v>303</v>
+        <v>73</v>
       </c>
       <c r="L19">
-        <v>10156</v>
+        <v>3363</v>
       </c>
       <c r="M19">
-        <v>11038</v>
+        <v>3705</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>87</v>
+      <c r="A20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>755</v>
+        <v>299</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>756</v>
+        <v>300</v>
       </c>
       <c r="F20">
-        <v>132</v>
+        <v>703</v>
       </c>
       <c r="G20">
-        <v>2.25718194254446E-2</v>
+        <v>4.6590231294320363E-2</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20">
-        <v>15764</v>
+        <v>47023</v>
       </c>
       <c r="J20">
-        <v>91</v>
+        <v>382</v>
       </c>
       <c r="K20">
-        <v>93</v>
+        <v>238</v>
       </c>
       <c r="L20">
-        <v>5848</v>
+        <v>15089</v>
       </c>
       <c r="M20">
-        <v>6032</v>
+        <v>15709</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>538</v>
+      <c r="A21" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>539</v>
+        <v>223</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>755</v>
+        <v>224</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>756</v>
+        <v>225</v>
       </c>
       <c r="F21">
-        <v>129</v>
+        <v>733</v>
       </c>
       <c r="G21">
-        <v>1.3188835497392901E-2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0</v>
+        <v>0.1066647264260768</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
       </c>
       <c r="I21">
-        <v>25874</v>
+        <v>16494</v>
       </c>
       <c r="J21">
-        <v>229</v>
+        <v>329</v>
       </c>
       <c r="K21">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L21">
-        <v>9781</v>
+        <v>6872</v>
       </c>
       <c r="M21">
-        <v>10109</v>
+        <v>7302</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>755</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>756</v>
+        <v>286</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>287</v>
       </c>
       <c r="F22">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="G22">
-        <v>6.2439136163143722E-3</v>
-      </c>
-      <c r="H22" s="12">
         <v>0</v>
       </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
       <c r="I22">
-        <v>46430</v>
+        <v>8969</v>
       </c>
       <c r="J22">
-        <v>384</v>
+        <v>176</v>
       </c>
       <c r="K22">
-        <v>209</v>
+        <v>47</v>
       </c>
       <c r="L22">
-        <v>17457</v>
+        <v>4274</v>
       </c>
       <c r="M22">
-        <v>18050</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" t="s">
-        <v>755</v>
+      <c r="A23" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>753</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="F23">
-        <v>261</v>
-      </c>
-      <c r="G23">
-        <v>3.076741718731581E-2</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>38119</v>
-      </c>
-      <c r="J23">
-        <v>392</v>
-      </c>
-      <c r="K23">
-        <v>296</v>
-      </c>
-      <c r="L23" s="5">
-        <v>8484</v>
-      </c>
-      <c r="M23" s="5">
-        <v>9172</v>
+        <v>754</v>
+      </c>
+      <c r="F23" s="20">
+        <v>846</v>
+      </c>
+      <c r="G23" s="20">
+        <v>4.4613194114855252E-2</v>
+      </c>
+      <c r="H23" s="20">
+        <v>2</v>
+      </c>
+      <c r="I23" s="20">
+        <v>80820</v>
+      </c>
+      <c r="J23" s="20">
+        <v>950</v>
+      </c>
+      <c r="K23" s="20">
+        <v>445</v>
+      </c>
+      <c r="L23" s="20">
+        <v>18963</v>
+      </c>
+      <c r="M23" s="20">
+        <v>20358</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>340</v>
+        <v>269</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F24">
-        <v>111</v>
+        <v>195</v>
       </c>
       <c r="G24">
-        <v>1.261363636363636E-2</v>
-      </c>
-      <c r="H24" s="6">
+        <v>4.2511445389143233E-2</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>11736</v>
+      </c>
+      <c r="J24">
+        <v>416</v>
+      </c>
+      <c r="K24">
+        <v>130</v>
+      </c>
+      <c r="L24">
+        <v>4587</v>
+      </c>
+      <c r="M24">
+        <v>5133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="F25" s="15">
+        <v>301</v>
+      </c>
+      <c r="G25" s="15">
+        <v>5.8950254602428517E-2</v>
+      </c>
+      <c r="H25" s="15">
+        <v>1</v>
+      </c>
+      <c r="I25" s="15">
+        <v>15911</v>
+      </c>
+      <c r="J25" s="15">
+        <v>232</v>
+      </c>
+      <c r="K25" s="15">
+        <v>119</v>
+      </c>
+      <c r="L25" s="15">
+        <v>5106</v>
+      </c>
+      <c r="M25" s="15">
+        <v>5457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>757</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="F26" s="20">
+        <v>178</v>
+      </c>
+      <c r="G26" s="20">
+        <v>2.5872093023255809E-2</v>
+      </c>
+      <c r="H26" s="20">
         <v>0</v>
       </c>
-      <c r="I24">
-        <v>37780</v>
-      </c>
-      <c r="J24">
-        <v>211</v>
-      </c>
-      <c r="K24">
-        <v>153</v>
-      </c>
-      <c r="L24">
-        <v>8800</v>
-      </c>
-      <c r="M24">
-        <v>9164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
-        <v>755</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="F25">
-        <v>232</v>
-      </c>
-      <c r="G25">
-        <v>3.0382399161864849E-2</v>
-      </c>
-      <c r="H25" s="3">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>17748</v>
-      </c>
-      <c r="J25">
-        <v>170</v>
-      </c>
-      <c r="K25">
-        <v>79</v>
-      </c>
-      <c r="L25">
-        <v>7636</v>
-      </c>
-      <c r="M25">
-        <v>7885</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s">
-        <v>755</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="F26">
-        <v>149</v>
-      </c>
-      <c r="G26">
-        <v>1.7626878031468118E-2</v>
-      </c>
-      <c r="H26" s="6">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>27942</v>
-      </c>
-      <c r="J26">
-        <v>279</v>
-      </c>
-      <c r="K26">
-        <v>167</v>
-      </c>
-      <c r="L26">
-        <v>8453</v>
-      </c>
-      <c r="M26">
-        <v>8899</v>
+      <c r="I26" s="20">
+        <v>16625</v>
+      </c>
+      <c r="J26" s="20">
+        <v>236</v>
+      </c>
+      <c r="K26" s="20">
+        <v>114</v>
+      </c>
+      <c r="L26" s="20">
+        <v>6880</v>
+      </c>
+      <c r="M26" s="20">
+        <v>7230</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>755</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="F27" s="20">
-        <v>1384</v>
-      </c>
-      <c r="G27" s="20">
-        <v>1.7393708605110029E-2</v>
-      </c>
-      <c r="H27" s="23">
-        <v>0</v>
-      </c>
-      <c r="I27" s="20">
-        <v>328134</v>
-      </c>
-      <c r="J27" s="20">
-        <v>2831</v>
-      </c>
-      <c r="K27" s="20">
-        <v>2058</v>
-      </c>
-      <c r="L27" s="20">
-        <v>79569</v>
-      </c>
-      <c r="M27" s="20">
-        <v>84458</v>
+      <c r="A27" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27">
+        <v>859</v>
+      </c>
+      <c r="G27">
+        <v>0.1598139534883721</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>15743</v>
+      </c>
+      <c r="J27">
+        <v>171</v>
+      </c>
+      <c r="K27">
+        <v>131</v>
+      </c>
+      <c r="L27">
+        <v>5375</v>
+      </c>
+      <c r="M27">
+        <v>5677</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>289</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>744</v>
-      </c>
-      <c r="F28" s="17">
-        <v>319</v>
-      </c>
-      <c r="G28" s="17">
-        <v>6.8308351177730195E-2</v>
-      </c>
-      <c r="H28" s="17">
-        <v>2</v>
-      </c>
-      <c r="I28" s="17">
-        <v>12970</v>
-      </c>
-      <c r="J28" s="17">
-        <v>209</v>
-      </c>
-      <c r="K28" s="17">
-        <v>92</v>
-      </c>
-      <c r="L28" s="17">
-        <v>4670</v>
-      </c>
-      <c r="M28" s="17">
-        <v>4971</v>
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28">
+        <v>286</v>
+      </c>
+      <c r="G28">
+        <v>0.13185799907791609</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>6922</v>
+      </c>
+      <c r="J28">
+        <v>147</v>
+      </c>
+      <c r="K28">
+        <v>68</v>
+      </c>
+      <c r="L28">
+        <v>2169</v>
+      </c>
+      <c r="M28">
+        <v>2384</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>608</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>609</v>
+        <v>301</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>290</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>744</v>
+        <v>303</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>304</v>
       </c>
       <c r="F29">
-        <v>155</v>
+        <v>1091</v>
       </c>
       <c r="G29">
-        <v>6.9851284362325378E-2</v>
-      </c>
-      <c r="H29" s="6">
+        <v>3.714421898406646E-2</v>
+      </c>
+      <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>5031</v>
+        <v>76783</v>
       </c>
       <c r="J29">
-        <v>69</v>
+        <v>456</v>
       </c>
       <c r="K29">
-        <v>43</v>
+        <v>335</v>
       </c>
       <c r="L29">
-        <v>2219</v>
+        <v>29372</v>
       </c>
       <c r="M29">
-        <v>2331</v>
+        <v>30163</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>736</v>
+        <v>262</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>737</v>
+        <v>263</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>290</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>744</v>
+        <v>303</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>304</v>
       </c>
       <c r="F30">
-        <v>149</v>
+        <v>263</v>
       </c>
       <c r="G30">
-        <v>4.4305679452869458E-2</v>
+        <v>2.5073886929163881E-2</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>10945</v>
+        <v>41646</v>
       </c>
       <c r="J30">
-        <v>269</v>
+        <v>586</v>
       </c>
       <c r="K30">
-        <v>73</v>
+        <v>314</v>
       </c>
       <c r="L30">
-        <v>3363</v>
+        <v>10489</v>
       </c>
       <c r="M30">
-        <v>3705</v>
+        <v>11389</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>293</v>
+      <c r="A31" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>303</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F31" s="17">
-        <v>612</v>
-      </c>
-      <c r="G31" s="17">
-        <v>0.1310492505353319</v>
-      </c>
-      <c r="H31" s="17">
-        <v>3</v>
-      </c>
-      <c r="I31" s="17">
-        <v>12970</v>
-      </c>
-      <c r="J31" s="17">
+        <v>304</v>
+      </c>
+      <c r="F31" s="20">
+        <v>791</v>
+      </c>
+      <c r="G31" s="20">
+        <v>4.1712809154669621E-2</v>
+      </c>
+      <c r="H31" s="20">
+        <v>2</v>
+      </c>
+      <c r="I31" s="20">
+        <v>80820</v>
+      </c>
+      <c r="J31" s="20">
+        <v>950</v>
+      </c>
+      <c r="K31" s="20">
+        <v>445</v>
+      </c>
+      <c r="L31" s="20">
+        <v>18963</v>
+      </c>
+      <c r="M31" s="20">
+        <v>20358</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>303</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F32">
+        <v>337</v>
+      </c>
+      <c r="G32">
+        <v>0.11056430446194231</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>6237</v>
+      </c>
+      <c r="J32">
+        <v>123</v>
+      </c>
+      <c r="K32">
+        <v>42</v>
+      </c>
+      <c r="L32">
+        <v>3048</v>
+      </c>
+      <c r="M32">
+        <v>3213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>303</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F33">
+        <v>1105</v>
+      </c>
+      <c r="G33">
+        <v>8.4454295322531334E-2</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>44901</v>
+      </c>
+      <c r="J33">
+        <v>329</v>
+      </c>
+      <c r="K33">
         <v>209</v>
       </c>
-      <c r="K31" s="17">
-        <v>92</v>
-      </c>
-      <c r="L31" s="17">
-        <v>4670</v>
-      </c>
-      <c r="M31" s="17">
-        <v>4971</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" t="s">
-        <v>293</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F32">
-        <v>197</v>
-      </c>
-      <c r="G32">
-        <v>3.319292333614153E-2</v>
-      </c>
-      <c r="H32" s="11">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>11967</v>
-      </c>
-      <c r="J32">
-        <v>193</v>
-      </c>
-      <c r="K32">
-        <v>113</v>
-      </c>
-      <c r="L32">
-        <v>5935</v>
-      </c>
-      <c r="M32">
-        <v>6241</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F33" s="20">
-        <v>1168</v>
-      </c>
-      <c r="G33" s="20">
-        <v>0.1700393070315912</v>
-      </c>
-      <c r="H33" s="20">
-        <v>5</v>
-      </c>
-      <c r="I33" s="20">
-        <v>20443</v>
-      </c>
-      <c r="J33" s="20">
-        <v>297</v>
-      </c>
-      <c r="K33" s="20">
-        <v>142</v>
-      </c>
-      <c r="L33" s="20">
-        <v>6869</v>
-      </c>
-      <c r="M33" s="20">
-        <v>7308</v>
+      <c r="L33">
+        <v>13084</v>
+      </c>
+      <c r="M33">
+        <v>13622</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>313</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>51</v>
+        <v>314</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="F34">
-        <v>2536</v>
+        <v>357</v>
       </c>
       <c r="G34">
-        <v>0.25284147557328018</v>
-      </c>
-      <c r="H34" s="6">
-        <v>6</v>
+        <v>4.669718770438195E-2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>26781</v>
+        <v>29721</v>
       </c>
       <c r="J34">
-        <v>294</v>
+        <v>401</v>
       </c>
       <c r="K34">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="L34">
-        <v>10030</v>
+        <v>7645</v>
       </c>
       <c r="M34">
-        <v>10503</v>
+        <v>8220</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>143</v>
+      <c r="A35" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="C35" t="s">
         <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="F35">
-        <v>914</v>
+        <v>3549</v>
       </c>
       <c r="G35">
-        <v>0.12309764309764309</v>
+        <v>7.8092681424107732E-2</v>
       </c>
       <c r="H35">
         <v>4</v>
       </c>
       <c r="I35">
-        <v>26031</v>
+        <v>148647</v>
       </c>
       <c r="J35">
-        <v>383</v>
+        <v>1007</v>
       </c>
       <c r="K35">
-        <v>208</v>
+        <v>784</v>
       </c>
       <c r="L35">
-        <v>7425</v>
+        <v>45446</v>
       </c>
       <c r="M35">
-        <v>8016</v>
+        <v>47237</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>297</v>
+        <v>182</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>298</v>
+        <v>183</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
       </c>
       <c r="D36" t="s">
+        <v>303</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F36">
+        <v>1488</v>
+      </c>
+      <c r="G36">
+        <v>4.9580167932826873E-2</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>102744</v>
+      </c>
+      <c r="J36">
+        <v>921</v>
+      </c>
+      <c r="K36">
+        <v>561</v>
+      </c>
+      <c r="L36">
+        <v>30012</v>
+      </c>
+      <c r="M36">
+        <v>31494</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>303</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F37">
+        <v>116</v>
+      </c>
+      <c r="G37">
+        <v>3.9375424304141211E-2</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>9975</v>
+      </c>
+      <c r="J37">
+        <v>258</v>
+      </c>
+      <c r="K37">
+        <v>64</v>
+      </c>
+      <c r="L37">
+        <v>2946</v>
+      </c>
+      <c r="M37">
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="F36">
-        <v>320</v>
-      </c>
-      <c r="G36">
-        <v>0.10606562810739149</v>
-      </c>
-      <c r="H36">
+      <c r="F38" s="17">
+        <v>612</v>
+      </c>
+      <c r="G38" s="17">
+        <v>0.1310492505353319</v>
+      </c>
+      <c r="H38" s="17">
         <v>3</v>
       </c>
-      <c r="I36">
-        <v>11803</v>
-      </c>
-      <c r="J36">
-        <v>156</v>
-      </c>
-      <c r="K36">
-        <v>69</v>
-      </c>
-      <c r="L36">
-        <v>3017</v>
-      </c>
-      <c r="M36">
-        <v>3242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>642</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" t="s">
-        <v>293</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F37">
-        <v>658</v>
-      </c>
-      <c r="G37">
-        <v>0.1275688251260178</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>13361</v>
-      </c>
-      <c r="J37">
-        <v>277</v>
-      </c>
-      <c r="K37">
-        <v>118</v>
-      </c>
-      <c r="L37">
-        <v>5158</v>
-      </c>
-      <c r="M37">
-        <v>5553</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>208</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="I38" s="17">
+        <v>12970</v>
+      </c>
+      <c r="J38" s="17">
         <v>209</v>
       </c>
-      <c r="C38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" t="s">
-        <v>299</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="F38">
-        <v>703</v>
-      </c>
-      <c r="G38">
-        <v>4.6590231294320363E-2</v>
-      </c>
-      <c r="H38">
-        <v>2</v>
-      </c>
-      <c r="I38">
-        <v>47023</v>
-      </c>
-      <c r="J38">
-        <v>382</v>
-      </c>
-      <c r="K38">
-        <v>238</v>
-      </c>
-      <c r="L38">
-        <v>15089</v>
-      </c>
-      <c r="M38">
-        <v>15709</v>
+      <c r="K38" s="17">
+        <v>92</v>
+      </c>
+      <c r="L38" s="17">
+        <v>4670</v>
+      </c>
+      <c r="M38" s="17">
+        <v>4971</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>223</v>
+        <v>291</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>225</v>
+        <v>293</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="F39">
-        <v>733</v>
+        <v>197</v>
       </c>
       <c r="G39">
-        <v>0.1066647264260768</v>
-      </c>
-      <c r="H39">
-        <v>3</v>
+        <v>3.319292333614153E-2</v>
+      </c>
+      <c r="H39" s="11">
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>16494</v>
+        <v>11967</v>
       </c>
       <c r="J39">
-        <v>329</v>
+        <v>193</v>
       </c>
       <c r="K39">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="L39">
-        <v>6872</v>
+        <v>5935</v>
       </c>
       <c r="M39">
-        <v>7302</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" t="s">
-        <v>745</v>
+      <c r="A40" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>293</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>746</v>
-      </c>
-      <c r="F40">
-        <v>214</v>
-      </c>
-      <c r="G40">
-        <v>5.1715804736587732E-2</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40">
-        <v>11900</v>
-      </c>
-      <c r="J40">
-        <v>336</v>
-      </c>
-      <c r="K40">
-        <v>124</v>
-      </c>
-      <c r="L40">
-        <v>4138</v>
-      </c>
-      <c r="M40">
-        <v>4598</v>
+        <v>294</v>
+      </c>
+      <c r="F40" s="20">
+        <v>1168</v>
+      </c>
+      <c r="G40" s="20">
+        <v>0.1700393070315912</v>
+      </c>
+      <c r="H40" s="20">
+        <v>5</v>
+      </c>
+      <c r="I40" s="20">
+        <v>20443</v>
+      </c>
+      <c r="J40" s="20">
+        <v>297</v>
+      </c>
+      <c r="K40" s="20">
+        <v>142</v>
+      </c>
+      <c r="L40" s="20">
+        <v>6869</v>
+      </c>
+      <c r="M40" s="20">
+        <v>7308</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>285</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>286</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>287</v>
+        <v>293</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="F41">
-        <v>150</v>
+        <v>2536</v>
       </c>
       <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
+        <v>0.25284147557328018</v>
+      </c>
+      <c r="H41" s="6">
+        <v>6</v>
       </c>
       <c r="I41">
-        <v>8969</v>
+        <v>26781</v>
       </c>
       <c r="J41">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="K41">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="L41">
-        <v>4274</v>
+        <v>10030</v>
       </c>
       <c r="M41">
-        <v>4497</v>
+        <v>10503</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>293</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F42">
+        <v>914</v>
+      </c>
+      <c r="G42">
+        <v>0.12309764309764309</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>26031</v>
+      </c>
+      <c r="J42">
+        <v>383</v>
+      </c>
+      <c r="K42">
+        <v>208</v>
+      </c>
+      <c r="L42">
+        <v>7425</v>
+      </c>
+      <c r="M42">
+        <v>8016</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>297</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>293</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F43">
+        <v>320</v>
+      </c>
+      <c r="G43">
+        <v>0.10606562810739149</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>11803</v>
+      </c>
+      <c r="J43">
+        <v>156</v>
+      </c>
+      <c r="K43">
+        <v>69</v>
+      </c>
+      <c r="L43">
+        <v>3017</v>
+      </c>
+      <c r="M43">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>642</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>293</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F44">
+        <v>658</v>
+      </c>
+      <c r="G44">
+        <v>0.1275688251260178</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>13361</v>
+      </c>
+      <c r="J44">
+        <v>277</v>
+      </c>
+      <c r="K44">
+        <v>118</v>
+      </c>
+      <c r="L44">
+        <v>5158</v>
+      </c>
+      <c r="M44">
+        <v>5553</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>745</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="F45">
+        <v>214</v>
+      </c>
+      <c r="G45">
+        <v>5.1715804736587732E-2</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>11900</v>
+      </c>
+      <c r="J45">
+        <v>336</v>
+      </c>
+      <c r="K45">
+        <v>124</v>
+      </c>
+      <c r="L45">
+        <v>4138</v>
+      </c>
+      <c r="M45">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>238</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" t="s">
-        <v>228</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="F42">
-        <v>217</v>
-      </c>
-      <c r="G42">
-        <v>4.9117247623358992E-2</v>
-      </c>
-      <c r="H42" s="6">
-        <v>1</v>
-      </c>
-      <c r="I42">
-        <v>15326</v>
-      </c>
-      <c r="J42">
-        <v>147</v>
-      </c>
-      <c r="K42">
-        <v>64</v>
-      </c>
-      <c r="L42">
-        <v>4418</v>
-      </c>
-      <c r="M42">
-        <v>4629</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" t="s">
-        <v>228</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="F43">
-        <v>151</v>
-      </c>
-      <c r="G43">
-        <v>3.476058931860037E-2</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43">
-        <v>11743</v>
-      </c>
-      <c r="J43">
-        <v>224</v>
-      </c>
-      <c r="K43">
-        <v>95</v>
-      </c>
-      <c r="L43">
-        <v>4344</v>
-      </c>
-      <c r="M43">
-        <v>4663</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" t="s">
-        <v>228</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="F44">
-        <v>99</v>
-      </c>
-      <c r="G44">
-        <v>2.0965692503176619E-2</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>9651</v>
-      </c>
-      <c r="J44">
-        <v>239</v>
-      </c>
-      <c r="K44">
-        <v>96</v>
-      </c>
-      <c r="L44">
-        <v>4722</v>
-      </c>
-      <c r="M44">
-        <v>5057</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>226</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" t="s">
-        <v>228</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="F45">
-        <v>134</v>
-      </c>
-      <c r="G45">
-        <v>1.7080943275971958E-2</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>20136</v>
-      </c>
-      <c r="J45">
-        <v>259</v>
-      </c>
-      <c r="K45">
-        <v>136</v>
-      </c>
-      <c r="L45">
-        <v>7845</v>
-      </c>
-      <c r="M45">
-        <v>8240</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
@@ -6097,77 +6097,77 @@
         <v>229</v>
       </c>
       <c r="F46">
-        <v>468</v>
+        <v>217</v>
       </c>
       <c r="G46">
-        <v>4.7025723472668812E-2</v>
-      </c>
-      <c r="H46">
+        <v>4.9117247623358992E-2</v>
+      </c>
+      <c r="H46" s="6">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>35526</v>
+        <v>15326</v>
       </c>
       <c r="J46">
-        <v>456</v>
+        <v>147</v>
       </c>
       <c r="K46">
-        <v>192</v>
+        <v>64</v>
       </c>
       <c r="L46">
-        <v>9952</v>
+        <v>4418</v>
       </c>
       <c r="M46">
-        <v>10600</v>
+        <v>4629</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="20" t="s">
+      <c r="A47" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
         <v>228</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F47" s="20">
-        <v>305</v>
-      </c>
-      <c r="G47" s="20">
-        <v>4.4331395348837212E-2</v>
-      </c>
-      <c r="H47" s="20">
+      <c r="F47">
+        <v>151</v>
+      </c>
+      <c r="G47">
+        <v>3.476058931860037E-2</v>
+      </c>
+      <c r="H47">
         <v>1</v>
       </c>
-      <c r="I47" s="20">
-        <v>16625</v>
-      </c>
-      <c r="J47" s="20">
+      <c r="I47">
+        <v>11743</v>
+      </c>
+      <c r="J47">
+        <v>224</v>
+      </c>
+      <c r="K47">
+        <v>95</v>
+      </c>
+      <c r="L47">
+        <v>4344</v>
+      </c>
+      <c r="M47">
+        <v>4663</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="K47" s="20">
-        <v>114</v>
-      </c>
-      <c r="L47" s="20">
-        <v>6880</v>
-      </c>
-      <c r="M47" s="20">
-        <v>7230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>242</v>
-      </c>
       <c r="B48" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
@@ -6179,36 +6179,36 @@
         <v>229</v>
       </c>
       <c r="F48">
-        <v>454</v>
+        <v>99</v>
       </c>
       <c r="G48">
-        <v>0.20626987732848709</v>
+        <v>2.0965692503176619E-2</v>
       </c>
       <c r="H48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>4571</v>
+        <v>9651</v>
       </c>
       <c r="J48">
-        <v>56</v>
+        <v>239</v>
       </c>
       <c r="K48">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="L48">
-        <v>2201</v>
+        <v>4722</v>
       </c>
       <c r="M48">
-        <v>2320</v>
+        <v>5057</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
@@ -6220,36 +6220,36 @@
         <v>229</v>
       </c>
       <c r="F49">
-        <v>449</v>
+        <v>134</v>
       </c>
       <c r="G49">
-        <v>6.1684297293584281E-2</v>
+        <v>1.7080943275971958E-2</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>18341</v>
+        <v>20136</v>
       </c>
       <c r="J49">
-        <v>351</v>
+        <v>259</v>
       </c>
       <c r="K49">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="L49">
-        <v>7279</v>
+        <v>7845</v>
       </c>
       <c r="M49">
-        <v>7781</v>
+        <v>8240</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>184</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>185</v>
+      <c r="A50" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
@@ -6261,77 +6261,77 @@
         <v>229</v>
       </c>
       <c r="F50">
-        <v>356</v>
+        <v>468</v>
       </c>
       <c r="G50">
-        <v>3.5646340242315007E-2</v>
+        <v>4.7025723472668812E-2</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>41689</v>
+        <v>35526</v>
       </c>
       <c r="J50">
-        <v>295</v>
+        <v>456</v>
       </c>
       <c r="K50">
-        <v>132</v>
+        <v>192</v>
       </c>
       <c r="L50">
-        <v>9987</v>
+        <v>9952</v>
       </c>
       <c r="M50">
-        <v>10414</v>
+        <v>10600</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C51" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="A51" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>228</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F51">
-        <v>137</v>
-      </c>
-      <c r="G51">
-        <v>3.0786516853932581E-2</v>
-      </c>
-      <c r="H51">
+      <c r="F51" s="20">
+        <v>305</v>
+      </c>
+      <c r="G51" s="20">
+        <v>4.4331395348837212E-2</v>
+      </c>
+      <c r="H51" s="20">
         <v>1</v>
       </c>
-      <c r="I51">
-        <v>10501</v>
-      </c>
-      <c r="J51">
-        <v>135</v>
-      </c>
-      <c r="K51">
-        <v>82</v>
-      </c>
-      <c r="L51">
-        <v>4450</v>
-      </c>
-      <c r="M51">
-        <v>4667</v>
+      <c r="I51" s="20">
+        <v>16625</v>
+      </c>
+      <c r="J51" s="20">
+        <v>236</v>
+      </c>
+      <c r="K51" s="20">
+        <v>114</v>
+      </c>
+      <c r="L51" s="20">
+        <v>6880</v>
+      </c>
+      <c r="M51" s="20">
+        <v>7230</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>181</v>
+      <c r="A52" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
@@ -6343,36 +6343,36 @@
         <v>229</v>
       </c>
       <c r="F52">
-        <v>109</v>
+        <v>454</v>
       </c>
       <c r="G52">
-        <v>1.2050856826976229E-2</v>
-      </c>
-      <c r="H52" s="5">
-        <v>0</v>
+        <v>0.20626987732848709</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
       </c>
       <c r="I52">
-        <v>18888</v>
+        <v>4571</v>
       </c>
       <c r="J52">
-        <v>272</v>
+        <v>56</v>
       </c>
       <c r="K52">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="L52">
-        <v>9045</v>
+        <v>2201</v>
       </c>
       <c r="M52">
-        <v>9453</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
@@ -6384,438 +6384,438 @@
         <v>229</v>
       </c>
       <c r="F53">
-        <v>497</v>
+        <v>449</v>
       </c>
       <c r="G53">
-        <v>0.1310999736217357</v>
-      </c>
-      <c r="H53" s="6">
+        <v>6.1684297293584281E-2</v>
+      </c>
+      <c r="H53">
         <v>2</v>
       </c>
       <c r="I53">
-        <v>8277</v>
+        <v>18341</v>
       </c>
       <c r="J53">
-        <v>196</v>
+        <v>351</v>
       </c>
       <c r="K53">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="L53">
-        <v>3791</v>
+        <v>7279</v>
       </c>
       <c r="M53">
-        <v>4088</v>
+        <v>7781</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>753</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>754</v>
-      </c>
-      <c r="F54" s="20">
-        <v>846</v>
-      </c>
-      <c r="G54" s="20">
-        <v>4.4613194114855252E-2</v>
-      </c>
-      <c r="H54" s="20">
-        <v>2</v>
-      </c>
-      <c r="I54" s="20">
-        <v>80820</v>
-      </c>
-      <c r="J54" s="20">
-        <v>950</v>
-      </c>
-      <c r="K54" s="20">
-        <v>445</v>
-      </c>
-      <c r="L54" s="20">
-        <v>18963</v>
-      </c>
-      <c r="M54" s="20">
-        <v>20358</v>
+      <c r="A54" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>228</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F54">
+        <v>356</v>
+      </c>
+      <c r="G54">
+        <v>3.5646340242315007E-2</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>41689</v>
+      </c>
+      <c r="J54">
+        <v>295</v>
+      </c>
+      <c r="K54">
+        <v>132</v>
+      </c>
+      <c r="L54">
+        <v>9987</v>
+      </c>
+      <c r="M54">
+        <v>10414</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>268</v>
+      <c r="A55" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>753</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>754</v>
+        <v>228</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="F55">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="G55">
-        <v>4.2511445389143233E-2</v>
+        <v>3.0786516853932581E-2</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>11736</v>
+        <v>10501</v>
       </c>
       <c r="J55">
-        <v>416</v>
+        <v>135</v>
       </c>
       <c r="K55">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="L55">
-        <v>4587</v>
+        <v>4450</v>
       </c>
       <c r="M55">
-        <v>5133</v>
+        <v>4667</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>404</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>405</v>
-      </c>
-      <c r="F56" s="15">
-        <v>301</v>
-      </c>
-      <c r="G56" s="15">
-        <v>5.8950254602428517E-2</v>
-      </c>
-      <c r="H56" s="15">
-        <v>1</v>
-      </c>
-      <c r="I56" s="15">
-        <v>15911</v>
-      </c>
-      <c r="J56" s="15">
-        <v>232</v>
-      </c>
-      <c r="K56" s="15">
-        <v>119</v>
-      </c>
-      <c r="L56" s="15">
-        <v>5106</v>
-      </c>
-      <c r="M56" s="15">
-        <v>5457</v>
+      <c r="A56" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>228</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F56">
+        <v>109</v>
+      </c>
+      <c r="G56">
+        <v>1.2050856826976229E-2</v>
+      </c>
+      <c r="H56" s="5">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>18888</v>
+      </c>
+      <c r="J56">
+        <v>272</v>
+      </c>
+      <c r="K56">
+        <v>136</v>
+      </c>
+      <c r="L56">
+        <v>9045</v>
+      </c>
+      <c r="M56">
+        <v>9453</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>240</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>228</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F57">
+        <v>497</v>
+      </c>
+      <c r="G57">
+        <v>0.1310999736217357</v>
+      </c>
+      <c r="H57" s="6">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>8277</v>
+      </c>
+      <c r="J57">
+        <v>196</v>
+      </c>
+      <c r="K57">
+        <v>101</v>
+      </c>
+      <c r="L57">
+        <v>3791</v>
+      </c>
+      <c r="M57">
+        <v>4088</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C57" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" t="s">
-        <v>104</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F57">
-        <v>171</v>
-      </c>
-      <c r="G57">
-        <v>4.4811320754716978E-2</v>
-      </c>
-      <c r="H57">
-        <v>1</v>
-      </c>
-      <c r="I57">
-        <v>17717</v>
-      </c>
-      <c r="J57">
-        <v>247</v>
-      </c>
-      <c r="K57">
-        <v>118</v>
-      </c>
-      <c r="L57">
-        <v>3816</v>
-      </c>
-      <c r="M57">
-        <v>4181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="15" t="s">
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
         <v>104</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F58" s="15">
-        <v>54</v>
-      </c>
-      <c r="G58" s="15">
-        <v>1.0575793184488839E-2</v>
-      </c>
-      <c r="H58" s="15">
-        <v>0</v>
-      </c>
-      <c r="I58" s="15">
-        <v>15911</v>
-      </c>
-      <c r="J58" s="15">
-        <v>232</v>
-      </c>
-      <c r="K58" s="15">
-        <v>119</v>
-      </c>
-      <c r="L58" s="15">
-        <v>5106</v>
-      </c>
-      <c r="M58" s="15">
-        <v>5457</v>
+      <c r="F58">
+        <v>171</v>
+      </c>
+      <c r="G58">
+        <v>4.4811320754716978E-2</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>17717</v>
+      </c>
+      <c r="J58">
+        <v>247</v>
+      </c>
+      <c r="K58">
+        <v>118</v>
+      </c>
+      <c r="L58">
+        <v>3816</v>
+      </c>
+      <c r="M58">
+        <v>4181</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B59" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="A59" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="15" t="s">
         <v>104</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="20">
-        <v>211</v>
-      </c>
-      <c r="G59" s="20">
-        <v>1.4432284541723669E-2</v>
-      </c>
-      <c r="H59" s="20">
+      <c r="F59" s="15">
+        <v>54</v>
+      </c>
+      <c r="G59" s="15">
+        <v>1.0575793184488839E-2</v>
+      </c>
+      <c r="H59" s="15">
         <v>0</v>
       </c>
-      <c r="I59" s="20">
-        <v>50600</v>
-      </c>
-      <c r="J59" s="20">
-        <v>325</v>
-      </c>
-      <c r="K59" s="20">
-        <v>195</v>
-      </c>
-      <c r="L59" s="20">
-        <v>14620</v>
-      </c>
-      <c r="M59" s="20">
-        <v>15140</v>
+      <c r="I59" s="15">
+        <v>15911</v>
+      </c>
+      <c r="J59" s="15">
+        <v>232</v>
+      </c>
+      <c r="K59" s="15">
+        <v>119</v>
+      </c>
+      <c r="L59" s="15">
+        <v>5106</v>
+      </c>
+      <c r="M59" s="15">
+        <v>5457</v>
       </c>
     </row>
     <row r="60" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="A60" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>104</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F60">
-        <v>529</v>
-      </c>
-      <c r="G60">
-        <v>7.2090487871354594E-2</v>
-      </c>
-      <c r="H60">
-        <v>2</v>
-      </c>
-      <c r="I60">
-        <v>23448</v>
-      </c>
-      <c r="J60">
-        <v>210</v>
-      </c>
-      <c r="K60">
-        <v>172</v>
-      </c>
-      <c r="L60">
-        <v>7338</v>
-      </c>
-      <c r="M60">
-        <v>7720</v>
+      <c r="F60" s="20">
+        <v>211</v>
+      </c>
+      <c r="G60" s="20">
+        <v>1.4432284541723669E-2</v>
+      </c>
+      <c r="H60" s="20">
+        <v>0</v>
+      </c>
+      <c r="I60" s="20">
+        <v>50600</v>
+      </c>
+      <c r="J60" s="20">
+        <v>325</v>
+      </c>
+      <c r="K60" s="20">
+        <v>195</v>
+      </c>
+      <c r="L60" s="20">
+        <v>14620</v>
+      </c>
+      <c r="M60" s="20">
+        <v>15140</v>
       </c>
     </row>
     <row r="61" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B61" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" s="20" t="s">
+      <c r="A61" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
         <v>104</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F61" s="20">
-        <v>1041</v>
-      </c>
-      <c r="G61" s="20">
-        <v>1.3082984579421629E-2</v>
-      </c>
-      <c r="H61" s="23">
-        <v>0</v>
-      </c>
-      <c r="I61" s="20">
-        <v>328134</v>
-      </c>
-      <c r="J61" s="20">
-        <v>2831</v>
-      </c>
-      <c r="K61" s="20">
-        <v>2058</v>
-      </c>
-      <c r="L61" s="20">
-        <v>79569</v>
-      </c>
-      <c r="M61" s="20">
-        <v>84458</v>
+      <c r="F61">
+        <v>529</v>
+      </c>
+      <c r="G61">
+        <v>7.2090487871354594E-2</v>
+      </c>
+      <c r="H61">
+        <v>2</v>
+      </c>
+      <c r="I61">
+        <v>23448</v>
+      </c>
+      <c r="J61">
+        <v>210</v>
+      </c>
+      <c r="K61">
+        <v>172</v>
+      </c>
+      <c r="L61">
+        <v>7338</v>
+      </c>
+      <c r="M61">
+        <v>7720</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C62" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="A62" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="20" t="s">
         <v>104</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="20">
+        <v>1041</v>
+      </c>
+      <c r="G62" s="20">
+        <v>1.3082984579421629E-2</v>
+      </c>
+      <c r="H62" s="23">
+        <v>0</v>
+      </c>
+      <c r="I62" s="20">
+        <v>328134</v>
+      </c>
+      <c r="J62" s="20">
+        <v>2831</v>
+      </c>
+      <c r="K62" s="20">
+        <v>2058</v>
+      </c>
+      <c r="L62" s="20">
+        <v>79569</v>
+      </c>
+      <c r="M62" s="20">
+        <v>84458</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>104</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63">
         <v>746</v>
       </c>
-      <c r="G62">
+      <c r="G63">
         <v>0.22709284627092849</v>
       </c>
-      <c r="H62">
+      <c r="H63">
         <v>4</v>
       </c>
-      <c r="I62">
+      <c r="I63">
         <v>8517</v>
       </c>
-      <c r="J62">
+      <c r="J63">
         <v>217</v>
       </c>
-      <c r="K62">
+      <c r="K63">
         <v>57</v>
       </c>
-      <c r="L62">
+      <c r="L63">
         <v>3285</v>
       </c>
-      <c r="M62">
+      <c r="M63">
         <v>3559</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="B63" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>757</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>373</v>
-      </c>
-      <c r="F63" s="20">
-        <v>178</v>
-      </c>
-      <c r="G63" s="20">
-        <v>2.5872093023255809E-2</v>
-      </c>
-      <c r="H63" s="20">
-        <v>0</v>
-      </c>
-      <c r="I63" s="20">
-        <v>16625</v>
-      </c>
-      <c r="J63" s="20">
-        <v>236</v>
-      </c>
-      <c r="K63" s="20">
-        <v>114</v>
-      </c>
-      <c r="L63" s="20">
-        <v>6880</v>
-      </c>
-      <c r="M63" s="20">
-        <v>7230</v>
       </c>
     </row>
   </sheetData>
@@ -6835,8 +6835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="A1:M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8657,8 +8657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G31" sqref="A1:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10354,7 +10354,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="E36" sqref="A1:M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15321,11 +15321,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>